<commit_message>
-Agent Performance Report Revision -Customer Upload Revison -Registration Revison -Customer List Revision
</commit_message>
<xml_diff>
--- a/public/import/Customer Upload.xlsx
+++ b/public/import/Customer Upload.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="105" windowWidth="18195" windowHeight="7740"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
   <si>
     <t>Title</t>
   </si>
@@ -76,12 +76,6 @@
     <t>Male</t>
   </si>
   <si>
-    <t>John</t>
-  </si>
-  <si>
-    <t>Kennedy</t>
-  </si>
-  <si>
     <t>QWE 100</t>
   </si>
   <si>
@@ -110,6 +104,24 @@
   </si>
   <si>
     <t>18-29</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>454dfdfasd34343</t>
+  </si>
+  <si>
+    <t>BRK</t>
+  </si>
+  <si>
+    <t>Juan</t>
+  </si>
+  <si>
+    <t>Dela Cruz</t>
+  </si>
+  <si>
+    <t>trackingurn</t>
   </si>
 </sst>
 </file>
@@ -485,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,9 +517,10 @@
     <col min="16" max="16" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -562,8 +575,14 @@
       <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="S1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -571,52 +590,58 @@
         <v>19</v>
       </c>
       <c r="C2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="G2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" t="s">
         <v>22</v>
       </c>
-      <c r="F2" t="s">
+      <c r="K2" t="s">
         <v>23</v>
       </c>
-      <c r="G2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="L2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>25</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="M2" t="s">
-        <v>27</v>
       </c>
       <c r="N2" s="3">
         <v>33982</v>
       </c>
       <c r="O2" t="s">
+        <v>26</v>
+      </c>
+      <c r="P2" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q2" t="s">
         <v>28</v>
       </c>
-      <c r="P2" t="s">
+      <c r="R2" t="s">
         <v>29</v>
       </c>
-      <c r="Q2" t="s">
-        <v>30</v>
-      </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>31</v>
+      </c>
+      <c r="T2" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>